<commit_message>
Adapt templates to work with latest release
</commit_message>
<xml_diff>
--- a/src/net/datenwerke/rs/samples/templates/jxls/jxlsdynamiclist/T_AGG_EMPLOYEE.xlsx
+++ b/src/net/datenwerke/rs/samples/templates/jxls/jxlsdynamiclist/T_AGG_EMPLOYEE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\tmp\jxls\jxlsdynamiclist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F193366-E08A-4315-AC15-55D729960074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D56CDE-3718-46DA-A310-A188A5084A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24075" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,13 +126,13 @@
     <t>Report template for Variant T_AGG_EMPLOYEE - Basis: Top Employee per Office</t>
   </si>
   <si>
-    <t>(Version: 1.0.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Last tested with: ReportServer 4.0.0) </t>
-  </si>
-  <si>
     <t>(Based on "T_AGG_EMPLOYEE - Basis: Top Employee per Office" DEMO Variant)</t>
+  </si>
+  <si>
+    <t>(Version: 1.0.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Last tested with: ReportServer 4.0.0-6053) </t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,17 +593,17 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>